<commit_message>
ablation study - No ATS model- 20Aug
</commit_message>
<xml_diff>
--- a/note.xlsx
+++ b/note.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913" refMode="R1C1"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="162">
   <si>
     <t>training note_ rain removal</t>
   </si>
@@ -273,13 +275,250 @@
   </si>
   <si>
     <t>fluctuate</t>
+  </si>
+  <si>
+    <t>using 2 loss: output loss + comb loss</t>
+  </si>
+  <si>
+    <t>Jun03_10-21</t>
+  </si>
+  <si>
+    <t>using instance norm in tranUnet, operation layer</t>
+  </si>
+  <si>
+    <t>Jun03_23-51</t>
+  </si>
+  <si>
+    <t>11.5-21.5</t>
+  </si>
+  <si>
+    <t>visualize not good - no fluctuate</t>
+  </si>
+  <si>
+    <t>Jun09-01-32</t>
+  </si>
+  <si>
+    <t>10.5-22</t>
+  </si>
+  <si>
+    <t>lr=2e-4</t>
+  </si>
+  <si>
+    <t>no instance norm in tranUnet</t>
+  </si>
+  <si>
+    <t>batch_size=2</t>
+  </si>
+  <si>
+    <t>Jun17-18-34</t>
+  </si>
+  <si>
+    <t>overfit at 50 epoch</t>
+  </si>
+  <si>
+    <t>Jun18-20-59</t>
+  </si>
+  <si>
+    <t>batch_size=8</t>
+  </si>
+  <si>
+    <t>using 3 loss: 2 loss + vgg loss</t>
+  </si>
+  <si>
+    <t>batch_size=4</t>
+  </si>
+  <si>
+    <t>Jun19-16-44</t>
+  </si>
+  <si>
+    <t>13-21</t>
+  </si>
+  <si>
+    <t>Jun21-19-45</t>
+  </si>
+  <si>
+    <t>comparison</t>
+  </si>
+  <si>
+    <t>PSNR</t>
+  </si>
+  <si>
+    <t>SSIM</t>
+  </si>
+  <si>
+    <t>+RCAN</t>
+  </si>
+  <si>
+    <t>visualization</t>
+  </si>
+  <si>
+    <t>visualiztion</t>
+  </si>
+  <si>
+    <t>good-visualize-consume much time</t>
+  </si>
+  <si>
+    <t>'</t>
+  </si>
+  <si>
+    <t>using 4 loss: 2 loss + vgg loss + ssim loss</t>
+  </si>
+  <si>
+    <t>Jun23-16-10</t>
+  </si>
+  <si>
+    <t>visulize &lt; Jun21 - consume nhieu time hon</t>
+  </si>
+  <si>
+    <t>Jun26-19-16</t>
+  </si>
+  <si>
+    <t>deeper in tranUnet (up to 512)</t>
+  </si>
+  <si>
+    <t>Jun28-12-24</t>
+  </si>
+  <si>
+    <t>tranUnet-1024</t>
+  </si>
+  <si>
+    <t>using patch=200, define up_feature in forward of Deraining model</t>
+  </si>
+  <si>
+    <t>ablation study - only clean layer</t>
+  </si>
+  <si>
+    <t>Jul07-16-34</t>
+  </si>
+  <si>
+    <t>visualize slightly good - no fluctuate</t>
+  </si>
+  <si>
+    <t>ok - not good as MSER feature</t>
+  </si>
+  <si>
+    <t>using 2 loss: output loss + vgg loss</t>
+  </si>
+  <si>
+    <t>using patch=200, define up_feature=image_size//16</t>
+  </si>
+  <si>
+    <t>lr=3e-5</t>
+  </si>
+  <si>
+    <t>visualize not good - slightly fluctuate</t>
+  </si>
+  <si>
+    <t>lr=5e-5</t>
+  </si>
+  <si>
+    <t>using 3 loss: output loss + vgg + ssim</t>
+  </si>
+  <si>
+    <t>overfit after 100 epoch</t>
+  </si>
+  <si>
+    <t>not satisfy</t>
+  </si>
+  <si>
+    <t>lr=5e-5, decay = 30 is best for 4 loss</t>
+  </si>
+  <si>
+    <t>lr=5e-5, decay = 100, 4 loss: output loss+vgg+ssim+edge</t>
+  </si>
+  <si>
+    <t>overfit at 100 epoch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 RG </t>
+  </si>
+  <si>
+    <t>heavy rain 2019_only_HR</t>
+  </si>
+  <si>
+    <t>heavy_rain_2019_LR+RCAN</t>
+  </si>
+  <si>
+    <t>NOTE</t>
+  </si>
+  <si>
+    <t>data_v4</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>LR - high result</t>
+  </si>
+  <si>
+    <t>test_with_train_param_v5 - 22.67 - 0.75550</t>
+  </si>
+  <si>
+    <t>Jul11-08-48</t>
+  </si>
+  <si>
+    <t>Jul13-16-13</t>
+  </si>
+  <si>
+    <t>Jul26-23-10</t>
+  </si>
+  <si>
+    <t>Jul28-20-02</t>
+  </si>
+  <si>
+    <t>lr=5e-5, decay=100, 4 loss=output loss + ssim+loss edge+loss stage1</t>
+  </si>
+  <si>
+    <t>separated mul_feat + add_feat</t>
+  </si>
+  <si>
+    <t>my result</t>
+  </si>
+  <si>
+    <t>Heavy_rain_2019 + RCAN</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>PreNet+RCAN</t>
+  </si>
+  <si>
+    <t>RESCAN + RCAN</t>
+  </si>
+  <si>
+    <t>SPANet+RCAN</t>
+  </si>
+  <si>
+    <t>DID-MDN_pretrained+RCAN</t>
+  </si>
+  <si>
+    <t>0.75550</t>
+  </si>
+  <si>
+    <t>SPANet(2019)+RCAN</t>
+  </si>
+  <si>
+    <t>PreNet(2019)+RCAN</t>
+  </si>
+  <si>
+    <t>RESCAN(2018) + RCAN</t>
+  </si>
+  <si>
+    <t>DID-MDN(2018)+RCAN</t>
+  </si>
+  <si>
+    <t>DID-MDN_epoch99+RCAN</t>
+  </si>
+  <si>
+    <t>DID-MDN_epoch49+RCAN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,13 +541,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -323,7 +582,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -340,12 +599,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView topLeftCell="F28" workbookViewId="0">
+      <selection activeCell="T45" sqref="T45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,40 +924,40 @@
     <col min="6" max="6" width="18.140625" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" customWidth="1"/>
     <col min="9" max="9" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="17.140625" customWidth="1"/>
-    <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" style="1" customWidth="1"/>
+    <col min="10" max="13" width="17.140625" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:16" s="7" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-    </row>
-    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M5" s="1" t="s">
+    <row r="4" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -685,14 +967,14 @@
       <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -708,17 +990,17 @@
       <c r="E7" t="s">
         <v>10</v>
       </c>
-      <c r="L7" t="s">
+      <c r="N7" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N7" t="s">
+      <c r="P7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
@@ -734,17 +1016,17 @@
       <c r="E8" t="s">
         <v>17</v>
       </c>
-      <c r="L8" t="s">
+      <c r="N8" t="s">
         <v>18</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N8" t="s">
+      <c r="P8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -760,11 +1042,11 @@
       <c r="E9" t="s">
         <v>11</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="O9" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -783,14 +1065,14 @@
       <c r="F10" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="1">
+      <c r="O10" s="1">
         <v>13.5</v>
       </c>
-      <c r="N10" t="s">
+      <c r="P10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -809,17 +1091,17 @@
       <c r="F11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L11" t="s">
+      <c r="N11" t="s">
         <v>23</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="O11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N11" t="s">
+      <c r="P11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -844,17 +1126,17 @@
       <c r="H12" t="s">
         <v>28</v>
       </c>
-      <c r="L12" t="s">
+      <c r="N12" t="s">
         <v>38</v>
       </c>
-      <c r="M12" s="5" t="s">
+      <c r="O12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="N12" t="s">
+      <c r="P12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -879,17 +1161,17 @@
       <c r="H13" t="s">
         <v>28</v>
       </c>
-      <c r="L13" t="s">
+      <c r="N13" t="s">
         <v>39</v>
       </c>
-      <c r="M13" s="5" t="s">
+      <c r="O13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="N13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -917,14 +1199,14 @@
       <c r="I14" t="s">
         <v>29</v>
       </c>
-      <c r="L14" t="s">
+      <c r="N14" t="s">
         <v>34</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="O14" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -952,17 +1234,17 @@
       <c r="I15" t="s">
         <v>30</v>
       </c>
-      <c r="L15" t="s">
+      <c r="N15" t="s">
         <v>31</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="O15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N15" t="s">
+      <c r="P15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>40</v>
       </c>
@@ -990,14 +1272,14 @@
       <c r="I16" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L16" t="s">
+      <c r="N16" t="s">
         <v>41</v>
       </c>
-      <c r="M16" s="5" t="s">
+      <c r="O16" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>40</v>
       </c>
@@ -1025,14 +1307,14 @@
       <c r="I17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L17" t="s">
+      <c r="N17" t="s">
         <v>45</v>
       </c>
-      <c r="M17" s="5" t="s">
+      <c r="O17" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>40</v>
       </c>
@@ -1052,17 +1334,17 @@
         <v>51</v>
       </c>
       <c r="G18" s="6"/>
-      <c r="L18" t="s">
+      <c r="N18" t="s">
         <v>48</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="O18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="N18" t="s">
+      <c r="P18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>40</v>
       </c>
@@ -1081,17 +1363,17 @@
       <c r="F19" t="s">
         <v>50</v>
       </c>
-      <c r="L19" t="s">
+      <c r="N19" t="s">
         <v>47</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="O19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="N19" t="s">
+      <c r="P19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>52</v>
       </c>
@@ -1101,42 +1383,42 @@
       <c r="J20" t="s">
         <v>53</v>
       </c>
-      <c r="L20" t="s">
+      <c r="N20" t="s">
         <v>54</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="O20" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>52</v>
       </c>
       <c r="F21" t="s">
         <v>51</v>
       </c>
-      <c r="M21" s="1">
+      <c r="O21" s="1">
         <v>11.5</v>
       </c>
-      <c r="N21" s="3" t="s">
+      <c r="P21" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
         <v>62</v>
       </c>
       <c r="J22" t="s">
         <v>59</v>
       </c>
-      <c r="L22" t="s">
+      <c r="N22" t="s">
         <v>58</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="O22" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>40</v>
       </c>
@@ -1167,17 +1449,17 @@
       <c r="J23" t="s">
         <v>63</v>
       </c>
-      <c r="L23" t="s">
+      <c r="N23" t="s">
         <v>64</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="O23" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="N23" t="s">
+      <c r="P23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>40</v>
       </c>
@@ -1211,77 +1493,406 @@
       <c r="K24" t="s">
         <v>66</v>
       </c>
-      <c r="L24" t="s">
+      <c r="N24" t="s">
         <v>71</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="O24" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="N24" t="s">
+      <c r="P24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
         <v>68</v>
       </c>
-      <c r="L25" t="s">
+      <c r="N25" t="s">
         <v>70</v>
       </c>
-      <c r="M25" s="1">
+      <c r="O25" s="1">
         <v>19</v>
       </c>
-      <c r="N25" t="s">
+      <c r="P25" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
         <v>72</v>
       </c>
-      <c r="L26" t="s">
+      <c r="N26" t="s">
         <v>73</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="O26" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A27" s="9" t="s">
+    <row r="27" spans="1:16" ht="21" x14ac:dyDescent="0.35">
+      <c r="A27" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
         <v>76</v>
       </c>
-      <c r="L28" t="s">
+      <c r="N28" t="s">
         <v>75</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="O28" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="O28" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H29" t="s">
         <v>79</v>
       </c>
-      <c r="L29" t="s">
+      <c r="N29" t="s">
         <v>80</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="O29" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="N29" t="s">
+      <c r="P29" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H30" t="s">
+        <v>79</v>
+      </c>
+      <c r="I30" t="s">
+        <v>83</v>
+      </c>
+      <c r="N30" t="s">
+        <v>84</v>
+      </c>
+      <c r="P30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>79</v>
+      </c>
+      <c r="J31" t="s">
+        <v>85</v>
+      </c>
+      <c r="N31" t="s">
+        <v>86</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>79</v>
+      </c>
+      <c r="N32" t="s">
+        <v>89</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="P32" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>91</v>
+      </c>
+      <c r="J33" t="s">
+        <v>92</v>
+      </c>
+      <c r="K33" t="s">
+        <v>93</v>
+      </c>
+      <c r="N33" t="s">
+        <v>94</v>
+      </c>
+      <c r="O33" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="P33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>79</v>
+      </c>
+      <c r="K34" t="s">
+        <v>97</v>
+      </c>
+      <c r="N34" t="s">
+        <v>96</v>
+      </c>
+      <c r="O34" s="1">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="35" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H35" t="s">
+        <v>79</v>
+      </c>
+      <c r="I35" t="s">
+        <v>98</v>
+      </c>
+      <c r="K35" t="s">
+        <v>99</v>
+      </c>
+      <c r="N35" t="s">
+        <v>100</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="P35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H36" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="N36" t="s">
+        <v>102</v>
+      </c>
+      <c r="O36" s="1">
+        <v>21.3</v>
+      </c>
+      <c r="P36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H37" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I37" t="s">
+        <v>111</v>
+      </c>
+      <c r="K37" t="s">
+        <v>93</v>
+      </c>
+      <c r="N37" t="s">
+        <v>112</v>
+      </c>
+      <c r="O37" s="1">
+        <v>18</v>
+      </c>
+      <c r="P37" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H38" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K38" t="s">
+        <v>99</v>
+      </c>
+      <c r="L38" t="s">
+        <v>118</v>
+      </c>
+      <c r="N38" t="s">
+        <v>114</v>
+      </c>
+      <c r="O38" s="1">
+        <v>19.5</v>
+      </c>
+      <c r="P38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H39" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="J39" t="s">
+        <v>115</v>
+      </c>
+      <c r="K39" t="s">
+        <v>99</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M39" s="6"/>
+      <c r="N39" t="s">
+        <v>116</v>
+      </c>
+      <c r="O39" s="1">
+        <v>22.5</v>
+      </c>
+      <c r="P39" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40" spans="8:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="J40" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="K40" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="L40" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="N40" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="O40" s="12">
+        <v>18</v>
+      </c>
+      <c r="P40" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H41" t="s">
+        <v>125</v>
+      </c>
+      <c r="I41" t="s">
+        <v>123</v>
+      </c>
+      <c r="J41" t="s">
+        <v>117</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="L41" t="s">
+        <v>124</v>
+      </c>
+      <c r="N41" t="s">
+        <v>142</v>
+      </c>
+      <c r="O41" s="1">
+        <v>21.5</v>
+      </c>
+      <c r="P41" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H42" t="s">
+        <v>127</v>
+      </c>
+      <c r="I42" t="s">
+        <v>128</v>
+      </c>
+      <c r="J42" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K42" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="L42" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="M42" s="6"/>
+      <c r="N42" t="s">
+        <v>143</v>
+      </c>
+      <c r="O42" s="1">
+        <v>22</v>
+      </c>
+      <c r="P42" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
+        <v>131</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="L43" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="M43" s="6"/>
+      <c r="O43" s="1">
+        <v>22</v>
+      </c>
+      <c r="P43" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H44" t="s">
+        <v>132</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="K44" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="L44" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="M44" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="N44" t="s">
+        <v>144</v>
+      </c>
+      <c r="O44" s="1">
+        <v>22</v>
+      </c>
+      <c r="P44" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="H45" t="s">
+        <v>146</v>
+      </c>
+      <c r="M45" t="s">
+        <v>147</v>
+      </c>
+      <c r="N45" t="s">
+        <v>145</v>
+      </c>
+      <c r="O45" s="1">
+        <v>24.8</v>
+      </c>
+      <c r="R45" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1292,4 +1903,312 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="2" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="H4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5">
+        <v>20.755490000000002</v>
+      </c>
+      <c r="C5">
+        <v>0.78220000000000001</v>
+      </c>
+      <c r="E5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F5" t="s">
+        <v>139</v>
+      </c>
+      <c r="H5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6">
+        <v>22.223379999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.84219999999999995</v>
+      </c>
+      <c r="D6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E6">
+        <v>21.214739999999999</v>
+      </c>
+      <c r="F6">
+        <v>0.70933000000000002</v>
+      </c>
+      <c r="H6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7">
+        <v>20.684660000000001</v>
+      </c>
+      <c r="C7">
+        <v>0.78373999999999999</v>
+      </c>
+      <c r="E7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8">
+        <v>22.00911</v>
+      </c>
+      <c r="C8">
+        <v>0.84026000000000001</v>
+      </c>
+      <c r="E8">
+        <v>21.019880000000001</v>
+      </c>
+      <c r="F8">
+        <v>0.70757999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9">
+        <v>19.184249999999999</v>
+      </c>
+      <c r="F9">
+        <v>0.64663000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="D10" t="s">
+        <v>150</v>
+      </c>
+      <c r="E10">
+        <v>21.940390000000001</v>
+      </c>
+      <c r="F10">
+        <v>0.74245000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>161</v>
+      </c>
+      <c r="E11">
+        <v>21.400860000000002</v>
+      </c>
+      <c r="F11">
+        <v>0.73711000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>151</v>
+      </c>
+      <c r="E12">
+        <v>16.26934</v>
+      </c>
+      <c r="F12">
+        <v>0.61931000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E13">
+        <v>21.72306</v>
+      </c>
+      <c r="F13">
+        <v>0.67481999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>153</v>
+      </c>
+      <c r="E14">
+        <v>20.46651</v>
+      </c>
+      <c r="F14">
+        <v>0.73619000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="13"/>
+      <c r="E17" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>148</v>
+      </c>
+      <c r="E18">
+        <v>22.678129999999999</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>149</v>
+      </c>
+      <c r="E19">
+        <v>21.019880000000001</v>
+      </c>
+      <c r="F19">
+        <v>0.70757999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>156</v>
+      </c>
+      <c r="E20">
+        <v>20.46651</v>
+      </c>
+      <c r="F20">
+        <v>0.73619000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>157</v>
+      </c>
+      <c r="E21">
+        <v>16.26934</v>
+      </c>
+      <c r="F21">
+        <v>0.61931000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>158</v>
+      </c>
+      <c r="E22">
+        <v>21.72306</v>
+      </c>
+      <c r="F22">
+        <v>0.67481999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>159</v>
+      </c>
+      <c r="E23">
+        <v>21.400860000000002</v>
+      </c>
+      <c r="F23">
+        <v>0.73711000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="B2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
extract feature from SCA_Unet, add#mul, norm[0,1]
</commit_message>
<xml_diff>
--- a/note.xlsx
+++ b/note.xlsx
@@ -12,11 +12,12 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7560" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Server91" sheetId="1" r:id="rId1"/>
+    <sheet name="Server65" sheetId="3" r:id="rId2"/>
+    <sheet name="Server66" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913" refMode="R1C1"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="268">
   <si>
     <t>training note_ rain removal</t>
   </si>
@@ -512,13 +513,331 @@
   </si>
   <si>
     <t>DID-MDN_epoch49+RCAN</t>
+  </si>
+  <si>
+    <t>lr=5e-5, decay=100, 3 loss= ssim+loss edge+loss stage1</t>
+  </si>
+  <si>
+    <t>Aug14-22-27</t>
+  </si>
+  <si>
+    <t>not good as Jul28</t>
+  </si>
+  <si>
+    <t>UMRL+RCAN</t>
+  </si>
+  <si>
+    <t>UMRL(2019)+RCAN</t>
+  </si>
+  <si>
+    <t>ablation</t>
+  </si>
+  <si>
+    <t>no ATS</t>
+  </si>
+  <si>
+    <t>no add</t>
+  </si>
+  <si>
+    <t>no mul</t>
+  </si>
+  <si>
+    <t>ablation study - no clean layer</t>
+  </si>
+  <si>
+    <t>ablation study - no add</t>
+  </si>
+  <si>
+    <t>ablation study - no mul</t>
+  </si>
+  <si>
+    <t>Aug26-10-57</t>
+  </si>
+  <si>
+    <t>Aug20-13-06</t>
+  </si>
+  <si>
+    <t>slightly not as good as Jul28</t>
+  </si>
+  <si>
+    <t>only Deraining</t>
+  </si>
+  <si>
+    <t>Deraining + SR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heavy_rain_2019 </t>
+  </si>
+  <si>
+    <t>SPANet(2019)</t>
+  </si>
+  <si>
+    <t>PreNet(2019)</t>
+  </si>
+  <si>
+    <t>UMRL(2019)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESCAN(2018) </t>
+  </si>
+  <si>
+    <t>DID-MDN(2018)</t>
+  </si>
+  <si>
+    <t>Semi(2019)</t>
+  </si>
+  <si>
+    <t>DDN</t>
+  </si>
+  <si>
+    <t>GMM</t>
+  </si>
+  <si>
+    <t>JCAS</t>
+  </si>
+  <si>
+    <t>Aug30-17-48</t>
+  </si>
+  <si>
+    <t>only deraining( no SR)</t>
+  </si>
+  <si>
+    <t>MSER-&gt; random point</t>
+  </si>
+  <si>
+    <t>sep09-18-35(sep11+sep13)</t>
+  </si>
+  <si>
+    <t>random point - SCA_Unet</t>
+  </si>
+  <si>
+    <t>sep19-10-56</t>
+  </si>
+  <si>
+    <t>MSER-SCA_Unet</t>
+  </si>
+  <si>
+    <t>good at syn but real image not good</t>
+  </si>
+  <si>
+    <t>sep24-17-41</t>
+  </si>
+  <si>
+    <t>loss=ssim+edge+loss_vgg+loss_stage1</t>
+  </si>
+  <si>
+    <t>loss=ssim+edge+loss_out+loss_vgg+loss_stage1</t>
+  </si>
+  <si>
+    <t>sep27-16-00</t>
+  </si>
+  <si>
+    <t>loss=loss_output+loss_edge+loss_vgg+loss_stage1</t>
+  </si>
+  <si>
+    <t>Oct02-15-12</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>loss= edge+vgg+stage1</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>16 thread</t>
+  </si>
+  <si>
+    <t>8 thread</t>
+  </si>
+  <si>
+    <t>Oct02-17-55</t>
+  </si>
+  <si>
+    <t>Oct02_17-35</t>
+  </si>
+  <si>
+    <t>RCDNet(2020)</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>MSPFN(2020)</t>
+  </si>
+  <si>
+    <t>loss=loss_out+loss_edge+loss_vgg+(loss_clean+loss_residual)</t>
+  </si>
+  <si>
+    <t>grid data-SCA_Unet</t>
+  </si>
+  <si>
+    <t>Oct09-12-34</t>
+  </si>
+  <si>
+    <t>add,mul not good</t>
+  </si>
+  <si>
+    <t>loss=loss_out+edge+vgg+loss_clean+res_add,mul</t>
+  </si>
+  <si>
+    <t>res=rain_img-free_img</t>
+  </si>
+  <si>
+    <t>Oct09_16-11</t>
+  </si>
+  <si>
+    <t>model = model-in-Oct09-S91</t>
+  </si>
+  <si>
+    <t>NEW MODEL IN ADD_LAYER + MUL_LAYER</t>
+  </si>
+  <si>
+    <t>3 operator_block in each layer(add, mul)</t>
+  </si>
+  <si>
+    <t>3 nhanh song song deu co kernel_size=7</t>
+  </si>
+  <si>
+    <t>consume much time, add-mul not good</t>
+  </si>
+  <si>
+    <t>add,mul layer-SCA</t>
+  </si>
+  <si>
+    <t>3 nhanh song song kernel=3.5.7</t>
+  </si>
+  <si>
+    <t>decease time, still add-mul not good</t>
+  </si>
+  <si>
+    <t>loss= loss_out+loss_edge+loss_vgg+(loss_clean+loss_add+loss_mul)</t>
+  </si>
+  <si>
+    <t>kernel=3,5,7</t>
+  </si>
+  <si>
+    <t>2 block operator in each mul, add_layer</t>
+  </si>
+  <si>
+    <t>sigmoid in add_block</t>
+  </si>
+  <si>
+    <t>check correct conv2,3,4=k3,5,7</t>
+  </si>
+  <si>
+    <t>them BatchNorm</t>
+  </si>
+  <si>
+    <t>not effective'</t>
+  </si>
+  <si>
+    <t>3*k7 &gt;&gt; k3,5,7 according to timing</t>
+  </si>
+  <si>
+    <t>no BN + loss(loss_add, mul_layer)</t>
+  </si>
+  <si>
+    <t>Oct12-13h58</t>
+  </si>
+  <si>
+    <t>1 operator block in add, mul_layer</t>
+  </si>
+  <si>
+    <t>them sigmoid in mul_layer</t>
+  </si>
+  <si>
+    <t>check correct conv 3*k7 -&gt; k,5,7</t>
+  </si>
+  <si>
+    <t>(loss=loss_add layer + loss_mul layer) and (khong co + in mul_layer)</t>
+  </si>
+  <si>
+    <t>oct12-14h26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">val </t>
+  </si>
+  <si>
+    <t>clean</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>mul</t>
+  </si>
+  <si>
+    <t>16-26</t>
+  </si>
+  <si>
+    <t>12-24</t>
+  </si>
+  <si>
+    <t>12-17</t>
+  </si>
+  <si>
+    <t>12-12</t>
+  </si>
+  <si>
+    <t>val</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>add(12-18), mul(12-12)</t>
+  </si>
+  <si>
+    <t>17-Oct-19-32</t>
+  </si>
+  <si>
+    <t>17-Oct-08-44</t>
+  </si>
+  <si>
+    <t>clean(25.9)-epoch50</t>
+  </si>
+  <si>
+    <t>add(17)-epoch30</t>
+  </si>
+  <si>
+    <t>only SCA-Unet</t>
+  </si>
+  <si>
+    <t>only add-layer</t>
+  </si>
+  <si>
+    <t>only mul-layer</t>
+  </si>
+  <si>
+    <t>16-Oct-21-13</t>
+  </si>
+  <si>
+    <t>mul(13)-epoch30</t>
+  </si>
+  <si>
+    <t>normalize = (0,1)</t>
+  </si>
+  <si>
+    <t>extract add, mul feature from SCA</t>
+  </si>
+  <si>
+    <t>add layer # mul_layer</t>
+  </si>
+  <si>
+    <t>Oct18-20h20</t>
+  </si>
+  <si>
+    <t>epoch173</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -549,6 +868,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -570,10 +896,67 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -582,7 +965,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -609,11 +992,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -624,10 +1025,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -908,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R45"/>
+  <dimension ref="A1:R69"/>
   <sheetViews>
-    <sheetView topLeftCell="F28" workbookViewId="0">
-      <selection activeCell="T45" sqref="T45"/>
+    <sheetView topLeftCell="F19" workbookViewId="0">
+      <selection activeCell="O53" sqref="O53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,16 +1330,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="7" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1529,14 +1929,14 @@
       </c>
     </row>
     <row r="27" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
@@ -1893,6 +2293,241 @@
       </c>
       <c r="R45" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="L46" t="s">
+        <v>171</v>
+      </c>
+      <c r="N46" t="s">
+        <v>175</v>
+      </c>
+      <c r="O46" s="1">
+        <v>24.8</v>
+      </c>
+      <c r="P46" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="47" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="L47" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="48" spans="8:18" x14ac:dyDescent="0.25">
+      <c r="L48" t="s">
+        <v>173</v>
+      </c>
+      <c r="N48" t="s">
+        <v>174</v>
+      </c>
+      <c r="O48" s="1">
+        <v>24.7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H49" t="s">
+        <v>162</v>
+      </c>
+      <c r="N49" t="s">
+        <v>163</v>
+      </c>
+      <c r="O49" s="1">
+        <v>24.3</v>
+      </c>
+      <c r="P49" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L50" t="s">
+        <v>190</v>
+      </c>
+      <c r="N50" t="s">
+        <v>189</v>
+      </c>
+      <c r="O50" s="1">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L51" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="N51" t="s">
+        <v>192</v>
+      </c>
+      <c r="O51" s="1">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L52" t="s">
+        <v>193</v>
+      </c>
+      <c r="N52" t="s">
+        <v>194</v>
+      </c>
+      <c r="O52" s="1">
+        <v>29</v>
+      </c>
+      <c r="R52" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H53" t="s">
+        <v>199</v>
+      </c>
+      <c r="L53" t="s">
+        <v>195</v>
+      </c>
+      <c r="N53" t="s">
+        <v>197</v>
+      </c>
+      <c r="O53" s="1">
+        <v>29</v>
+      </c>
+      <c r="P53" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H54" t="s">
+        <v>198</v>
+      </c>
+      <c r="L54" t="s">
+        <v>195</v>
+      </c>
+      <c r="N54" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H56" t="s">
+        <v>201</v>
+      </c>
+      <c r="K56" t="s">
+        <v>207</v>
+      </c>
+      <c r="L56" t="s">
+        <v>195</v>
+      </c>
+      <c r="N56" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K57" t="s">
+        <v>206</v>
+      </c>
+      <c r="N57" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H59" t="s">
+        <v>213</v>
+      </c>
+      <c r="L59" t="s">
+        <v>214</v>
+      </c>
+      <c r="N59" t="s">
+        <v>215</v>
+      </c>
+      <c r="P59" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A62" s="16" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>223</v>
+      </c>
+      <c r="H63" t="s">
+        <v>213</v>
+      </c>
+      <c r="L63" t="s">
+        <v>225</v>
+      </c>
+      <c r="P63" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>226</v>
+      </c>
+      <c r="P64" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="65" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>229</v>
+      </c>
+      <c r="H65" t="s">
+        <v>228</v>
+      </c>
+      <c r="N65" s="2">
+        <v>44116</v>
+      </c>
+      <c r="O65" s="1">
+        <v>26</v>
+      </c>
+      <c r="P65" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="67" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="L67" t="s">
+        <v>258</v>
+      </c>
+      <c r="N67" t="s">
+        <v>254</v>
+      </c>
+      <c r="O67" s="1">
+        <v>27</v>
+      </c>
+      <c r="P67" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="68" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="L68" t="s">
+        <v>259</v>
+      </c>
+      <c r="N68" t="s">
+        <v>255</v>
+      </c>
+      <c r="O68" s="1">
+        <v>19</v>
+      </c>
+      <c r="P68" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="69" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="L69" t="s">
+        <v>260</v>
+      </c>
+      <c r="N69" t="s">
+        <v>261</v>
+      </c>
+      <c r="O69" s="1">
+        <v>19</v>
+      </c>
+      <c r="P69" t="s">
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -1907,10 +2542,294 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="N8" sqref="N8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="13" width="9.140625" style="17"/>
+    <col min="16" max="16" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J1" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" t="s">
+        <v>211</v>
+      </c>
+      <c r="P1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>203</v>
+      </c>
+      <c r="I2" t="s">
+        <v>205</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="N2" t="s">
+        <v>104</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>44115</v>
+      </c>
+      <c r="B3" t="s">
+        <v>238</v>
+      </c>
+      <c r="O3" s="33"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>239</v>
+      </c>
+      <c r="O4" s="33"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>240</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="M5" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="O5" s="33"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>44116</v>
+      </c>
+      <c r="B6" t="s">
+        <v>241</v>
+      </c>
+      <c r="I6" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>44122</v>
+      </c>
+      <c r="B8" t="s">
+        <v>263</v>
+      </c>
+      <c r="I8" t="s">
+        <v>266</v>
+      </c>
+      <c r="N8">
+        <v>25.87</v>
+      </c>
+      <c r="O8">
+        <v>0.87065000000000003</v>
+      </c>
+      <c r="P8" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>265</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="25"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="20"/>
+    <col min="11" max="11" width="9.140625" style="21"/>
+    <col min="12" max="12" width="9.140625" style="22"/>
+    <col min="13" max="13" width="9.140625" style="23"/>
+    <col min="18" max="21" width="9.140625" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="24"/>
+      <c r="J1" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="K1" s="18"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="18"/>
+      <c r="O1" t="s">
+        <v>105</v>
+      </c>
+      <c r="P1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="I2" t="s">
+        <v>205</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="N2" t="s">
+        <v>211</v>
+      </c>
+      <c r="O2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="26">
+        <v>44106</v>
+      </c>
+      <c r="B3" t="s">
+        <v>204</v>
+      </c>
+      <c r="I3" t="s">
+        <v>209</v>
+      </c>
+      <c r="J3" s="20">
+        <v>27</v>
+      </c>
+      <c r="N3">
+        <v>24.8</v>
+      </c>
+      <c r="O3">
+        <v>0.82</v>
+      </c>
+      <c r="W3" s="29"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="26">
+        <v>44113</v>
+      </c>
+      <c r="B4" t="s">
+        <v>217</v>
+      </c>
+      <c r="I4" t="s">
+        <v>219</v>
+      </c>
+      <c r="W4" s="29"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>218</v>
+      </c>
+      <c r="W5" s="29"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="26">
+        <v>44115</v>
+      </c>
+      <c r="B8" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>232</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>233</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="26">
+        <v>44116</v>
+      </c>
+      <c r="B12" t="s">
+        <v>236</v>
+      </c>
+      <c r="I12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="W3:W5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1923,28 +2842,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="2" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
     </row>
@@ -1952,11 +2871,11 @@
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
@@ -1982,7 +2901,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="15" t="s">
         <v>135</v>
       </c>
       <c r="B5">
@@ -2002,7 +2921,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="15" t="s">
         <v>136</v>
       </c>
       <c r="B6">
@@ -2058,28 +2977,28 @@
         <v>0.70757999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+    <row r="9" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="15">
         <v>19.184249999999999</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="15">
         <v>0.64663000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="15">
         <v>21.940390000000001</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="15">
         <v>0.74245000000000005</v>
       </c>
     </row>
@@ -2096,110 +3015,309 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="E12">
-        <v>16.26934</v>
+        <v>21.235610000000001</v>
       </c>
       <c r="F12">
-        <v>0.61931000000000003</v>
+        <v>0.72990999999999995</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E13">
-        <v>21.72306</v>
+        <v>16.26934</v>
       </c>
       <c r="F13">
-        <v>0.67481999999999998</v>
+        <v>0.61931000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14">
+        <v>21.72306</v>
+      </c>
+      <c r="F14">
+        <v>0.67481999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>153</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <v>20.46651</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <v>0.73619000000000001</v>
       </c>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D17" s="13"/>
-      <c r="E17" s="13" t="s">
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D18" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F18" s="13" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
+      <c r="I18" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="J18" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
         <v>148</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <v>22.678129999999999</v>
       </c>
-      <c r="F18" s="19" t="s">
+      <c r="F19" s="14" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
+      <c r="I19" t="s">
+        <v>168</v>
+      </c>
+      <c r="J19">
+        <v>22.373729999999998</v>
+      </c>
+      <c r="K19">
+        <v>0.74816000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
         <v>149</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <v>21.019880000000001</v>
       </c>
-      <c r="F19">
+      <c r="F20">
         <v>0.70757999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
+      <c r="I20" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
         <v>156</v>
       </c>
-      <c r="E20">
+      <c r="E21">
         <v>20.46651</v>
       </c>
-      <c r="F20">
+      <c r="F21">
         <v>0.73619000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
+      <c r="I21" t="s">
+        <v>170</v>
+      </c>
+      <c r="J21">
+        <v>22.24155</v>
+      </c>
+      <c r="K21">
+        <v>0.74875999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
         <v>157</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <v>16.26934</v>
       </c>
-      <c r="F21">
+      <c r="F22">
         <v>0.61931000000000003</v>
       </c>
-    </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
+      <c r="I22" t="s">
+        <v>148</v>
+      </c>
+      <c r="J22">
+        <v>22.678129999999999</v>
+      </c>
+      <c r="K22">
+        <v>0.75549999999999995</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>166</v>
+      </c>
+      <c r="E23">
+        <v>21.235610000000001</v>
+      </c>
+      <c r="F23">
+        <v>0.72990999999999995</v>
+      </c>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
         <v>158</v>
       </c>
-      <c r="E22">
+      <c r="E24">
         <v>21.72306</v>
       </c>
-      <c r="F22">
+      <c r="F24">
         <v>0.67481999999999998</v>
       </c>
     </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
+    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
         <v>159</v>
       </c>
-      <c r="E23">
+      <c r="E25">
         <v>21.400860000000002</v>
       </c>
-      <c r="F23">
+      <c r="F25">
         <v>0.73711000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D28" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="E28" t="s">
+        <v>104</v>
+      </c>
+      <c r="F28" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>148</v>
+      </c>
+      <c r="E29">
+        <v>24.061060000000001</v>
+      </c>
+      <c r="F29">
+        <v>0.85787999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>179</v>
+      </c>
+      <c r="E30">
+        <v>20.684660000000001</v>
+      </c>
+      <c r="F30">
+        <v>0.78373999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>180</v>
+      </c>
+      <c r="E31">
+        <v>19.120180000000001</v>
+      </c>
+      <c r="F31">
+        <v>0.74614999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>181</v>
+      </c>
+      <c r="E32">
+        <v>17.825810000000001</v>
+      </c>
+      <c r="F32">
+        <v>0.71911000000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>182</v>
+      </c>
+      <c r="E33">
+        <v>21.58108</v>
+      </c>
+      <c r="F33">
+        <v>0.81655</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>183</v>
+      </c>
+      <c r="E34">
+        <v>21.773810000000001</v>
+      </c>
+      <c r="F34">
+        <v>0.70947000000000005</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>184</v>
+      </c>
+      <c r="E35">
+        <v>22.641310000000001</v>
+      </c>
+      <c r="F35">
+        <v>0.80749000000000004</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>185</v>
+      </c>
+      <c r="E36">
+        <v>18.883849999999999</v>
+      </c>
+      <c r="F36">
+        <v>0.64110999999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>210</v>
+      </c>
+      <c r="E37">
+        <v>22.435700000000001</v>
+      </c>
+      <c r="F37">
+        <v>0.81438999999999995</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>212</v>
+      </c>
+      <c r="E38">
+        <v>18.251390000000001</v>
+      </c>
+      <c r="F38">
+        <v>0.72633000000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>